<commit_message>
small ammendments  and results
</commit_message>
<xml_diff>
--- a/Traceback_Model/Input_Data/scenarios.xlsx
+++ b/Traceback_Model/Input_Data/scenarios.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sandra.Rudeloff\Documents\Pattern Comparison Project\Toy_Example\Traceback_Model\Input_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srude\Documents\Pattern Comparison Project\Toy_Example\Traceback_Model\Input_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4DD1347-CFBB-4BC9-9CC0-AC5ECEDEF099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6619412-9B95-449E-A6AD-3908CF7444BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population" sheetId="2" r:id="rId1"/>
@@ -36,8 +36,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="68">
   <si>
     <t xml:space="preserve">Population </t>
   </si>
@@ -235,13 +257,13 @@
     <t>Chain_Details</t>
   </si>
   <si>
-    <t>Population_details</t>
-  </si>
-  <si>
     <t>Outbreaks</t>
   </si>
   <si>
     <t>number of chains</t>
+  </si>
+  <si>
+    <t>Population</t>
   </si>
 </sst>
 </file>
@@ -251,7 +273,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,8 +320,22 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -326,8 +362,20 @@
         <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -591,11 +639,136 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -687,15 +860,76 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="8" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -705,68 +939,43 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1076,20 +1285,20 @@
   </sheetPr>
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E4"/>
+    <sheetView zoomScale="69" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="31" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" style="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>57</v>
       </c>
@@ -1106,7 +1315,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="24">
         <v>1</v>
       </c>
@@ -1119,7 +1328,7 @@
       <c r="D2" s="28"/>
       <c r="E2" s="29"/>
     </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24">
         <v>2</v>
       </c>
@@ -1136,7 +1345,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="24">
         <v>3</v>
       </c>
@@ -1149,98 +1358,150 @@
       <c r="D4" s="28"/>
       <c r="E4" s="29"/>
     </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="29"/>
-    </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="24"/>
+    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="24">
+        <v>4</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="24">
+        <v>20000</v>
+      </c>
+      <c r="D5" s="25">
+        <v>2.5</v>
+      </c>
+      <c r="E5" s="24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="24">
+        <v>5</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="24">
+        <v>20000</v>
+      </c>
       <c r="D6" s="28"/>
       <c r="E6" s="29"/>
     </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="29"/>
-    </row>
-    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="24"/>
-    </row>
-    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-    </row>
-    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="24"/>
-    </row>
-    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="24">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="24">
+        <v>20000</v>
+      </c>
+      <c r="D7" s="25">
+        <v>0.05</v>
+      </c>
+      <c r="E7" s="24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="24">
+        <v>7</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="24">
+        <v>5000</v>
+      </c>
+      <c r="D8" s="25">
+        <v>2.5</v>
+      </c>
+      <c r="E8" s="24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="24">
+        <v>8</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="24">
+        <v>20000</v>
+      </c>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+    </row>
+    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="24">
+        <v>9</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="24">
+        <v>20000</v>
+      </c>
+      <c r="D10" s="25">
+        <v>2.5</v>
+      </c>
+      <c r="E10" s="24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="24"/>
       <c r="B11" s="15"/>
       <c r="C11" s="24"/>
       <c r="D11" s="25"/>
       <c r="E11" s="24"/>
     </row>
-    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="24"/>
       <c r="B12" s="15"/>
       <c r="C12" s="24"/>
       <c r="D12" s="25"/>
       <c r="E12" s="29"/>
     </row>
-    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24"/>
       <c r="B13" s="15"/>
       <c r="C13" s="24"/>
       <c r="D13" s="25"/>
       <c r="E13" s="29"/>
     </row>
-    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="24"/>
       <c r="B14" s="15"/>
       <c r="C14" s="24"/>
       <c r="D14" s="25"/>
       <c r="E14" s="24"/>
     </row>
-    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="24"/>
       <c r="B15" s="15"/>
       <c r="C15" s="24"/>
       <c r="D15" s="25"/>
       <c r="E15" s="24"/>
     </row>
-    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="24"/>
       <c r="B16" s="15"/>
       <c r="C16" s="24"/>
       <c r="D16" s="25"/>
       <c r="E16" s="24"/>
     </row>
-    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="24"/>
       <c r="B17" s="15"/>
       <c r="C17" s="24"/>
       <c r="D17" s="28"/>
       <c r="E17" s="29"/>
     </row>
-    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="24"/>
       <c r="B18" s="15"/>
       <c r="C18" s="24"/>
@@ -1259,295 +1520,407 @@
   </sheetPr>
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" style="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" style="32" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" style="31" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.44140625" style="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="49" t="s">
+      <c r="G1" s="35" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="50">
-        <v>1</v>
-      </c>
-      <c r="B2" s="51">
-        <v>1</v>
-      </c>
-      <c r="C2" s="50">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="36">
+        <v>1</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="36">
         <v>10</v>
       </c>
-      <c r="D2" s="51" t="s">
+      <c r="D2" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="51" t="s">
+      <c r="E2" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="50">
+      <c r="F2" s="36">
         <v>10000</v>
       </c>
-      <c r="G2" s="52"/>
-    </row>
-    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="50">
+      <c r="G2" s="38"/>
+    </row>
+    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="36">
         <v>2</v>
       </c>
-      <c r="B3" s="51">
-        <v>1</v>
-      </c>
-      <c r="C3" s="50">
+      <c r="B3" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="36">
         <v>10</v>
       </c>
-      <c r="D3" s="51" t="s">
+      <c r="D3" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="51" t="s">
+      <c r="E3" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="50">
+      <c r="F3" s="36">
         <v>10000</v>
       </c>
-      <c r="G3" s="52"/>
-    </row>
-    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="50">
+      <c r="G3" s="38"/>
+    </row>
+    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="36">
         <v>3</v>
       </c>
-      <c r="B4" s="51">
-        <v>1</v>
-      </c>
-      <c r="C4" s="50">
+      <c r="B4" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="36">
         <v>10</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="E4" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="50">
+      <c r="F4" s="36">
         <v>10000</v>
       </c>
-      <c r="G4" s="52"/>
-    </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="50">
+      <c r="G4" s="38"/>
+    </row>
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="36">
         <v>3</v>
       </c>
-      <c r="B5" s="51">
-        <v>2</v>
-      </c>
-      <c r="C5" s="50">
+      <c r="B5" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="36">
         <v>5</v>
       </c>
-      <c r="D5" s="51" t="s">
+      <c r="D5" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="E5" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="50">
+      <c r="F5" s="36">
         <v>10000</v>
       </c>
-      <c r="G5" s="52"/>
-    </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="50"/>
-      <c r="B6" s="51"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="52"/>
-    </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="50"/>
-      <c r="B7" s="51"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="53"/>
-    </row>
-    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="50"/>
-      <c r="B8" s="51"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="52"/>
-    </row>
-    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
-      <c r="B9" s="51"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="52"/>
-    </row>
-    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
-      <c r="B10" s="51"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="52"/>
-    </row>
-    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
-      <c r="B11" s="51"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="52"/>
-    </row>
-    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
-      <c r="B12" s="51"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="52"/>
-    </row>
-    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="50"/>
-      <c r="B13" s="51"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="52"/>
-    </row>
-    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="50"/>
-      <c r="B14" s="51"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="52"/>
-    </row>
-    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="50"/>
-      <c r="B15" s="51"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="52"/>
-    </row>
-    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="50"/>
-      <c r="B16" s="51"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="52"/>
-    </row>
-    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="50"/>
-      <c r="B17" s="51"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="52"/>
-    </row>
-    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="50"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="50"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="52"/>
-    </row>
-    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="50"/>
-      <c r="B19" s="51"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="52"/>
-    </row>
-    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="50"/>
-      <c r="B20" s="51"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="52"/>
-    </row>
-    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="50"/>
-      <c r="B21" s="51"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="53"/>
-    </row>
-    <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="50"/>
-      <c r="B22" s="51"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="51"/>
-      <c r="F22" s="50"/>
-      <c r="G22" s="52"/>
-    </row>
-    <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="50"/>
-      <c r="B23" s="51"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="52"/>
-    </row>
-    <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="G5" s="39">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="36">
+        <v>4</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="36">
+        <v>10</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="36">
+        <v>10000</v>
+      </c>
+      <c r="G6" s="38"/>
+    </row>
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="36">
+        <v>4</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="36">
+        <v>5</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="36">
+        <v>10000</v>
+      </c>
+      <c r="G7" s="38"/>
+    </row>
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="36">
+        <v>5</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="36">
+        <v>10</v>
+      </c>
+      <c r="D8" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="36">
+        <v>10000</v>
+      </c>
+      <c r="G8" s="38"/>
+    </row>
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="36">
+        <v>6</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="36">
+        <v>10</v>
+      </c>
+      <c r="D9" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="36">
+        <v>10000</v>
+      </c>
+      <c r="G9" s="38"/>
+    </row>
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="36">
+        <v>6</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="36">
+        <v>5</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="36">
+        <v>10000</v>
+      </c>
+      <c r="G10" s="39">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="36">
+        <v>7</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="36">
+        <v>10</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="36">
+        <v>10000</v>
+      </c>
+      <c r="G11" s="38"/>
+    </row>
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="36">
+        <v>7</v>
+      </c>
+      <c r="B12" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="36">
+        <v>5</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="36">
+        <v>10000</v>
+      </c>
+      <c r="G12" s="38"/>
+    </row>
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="36">
+        <v>8</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="36">
+        <v>10</v>
+      </c>
+      <c r="D13" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="36">
+        <v>10000</v>
+      </c>
+      <c r="G13" s="38"/>
+    </row>
+    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="36">
+        <v>9</v>
+      </c>
+      <c r="B14" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="36">
+        <v>10</v>
+      </c>
+      <c r="D14" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="36">
+        <v>10000</v>
+      </c>
+      <c r="G14" s="38"/>
+    </row>
+    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="36"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="38"/>
+    </row>
+    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="36"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="38"/>
+    </row>
+    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="36"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="38"/>
+    </row>
+    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="36"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="38"/>
+    </row>
+    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="36"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="38"/>
+    </row>
+    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="36"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="38"/>
+    </row>
+    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="36"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="39"/>
+    </row>
+    <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="36"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="38"/>
+    </row>
+    <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="36"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="38"/>
+    </row>
+    <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1560,20 +1933,20 @@
   </sheetPr>
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E4"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" style="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" style="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.44140625" style="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>57</v>
       </c>
@@ -1590,7 +1963,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="24">
         <v>1</v>
       </c>
@@ -1607,7 +1980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24">
         <v>2</v>
       </c>
@@ -1624,7 +1997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="24">
         <v>3</v>
       </c>
@@ -1641,98 +2014,158 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-    </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-    </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-    </row>
-    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-    </row>
-    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-    </row>
-    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-    </row>
-    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="24">
+        <v>4</v>
+      </c>
+      <c r="B5" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="25">
+        <v>0.01</v>
+      </c>
+      <c r="D5" s="24">
+        <v>20</v>
+      </c>
+      <c r="E5" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="24">
+        <v>5</v>
+      </c>
+      <c r="B6" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="C6" s="25">
+        <v>0.01</v>
+      </c>
+      <c r="D6" s="24">
+        <v>10</v>
+      </c>
+      <c r="E6" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="24">
+        <v>6</v>
+      </c>
+      <c r="B7" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="C7" s="25">
+        <v>0.01</v>
+      </c>
+      <c r="D7" s="24">
+        <v>10</v>
+      </c>
+      <c r="E7" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="24">
+        <v>7</v>
+      </c>
+      <c r="B8" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="25">
+        <v>0.01</v>
+      </c>
+      <c r="D8" s="24">
+        <v>8</v>
+      </c>
+      <c r="E8" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="24">
+        <v>8</v>
+      </c>
+      <c r="B9" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="C9" s="25">
+        <v>0.01</v>
+      </c>
+      <c r="D9" s="24">
+        <v>7</v>
+      </c>
+      <c r="E9" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="24">
+        <v>9</v>
+      </c>
+      <c r="B10" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="C10" s="25">
+        <v>0.01</v>
+      </c>
+      <c r="D10" s="24">
+        <v>8</v>
+      </c>
+      <c r="E10" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="24"/>
       <c r="B11" s="25"/>
       <c r="C11" s="25"/>
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
     </row>
-    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="24"/>
       <c r="B12" s="25"/>
       <c r="C12" s="25"/>
       <c r="D12" s="24"/>
       <c r="E12" s="24"/>
     </row>
-    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24"/>
       <c r="B13" s="25"/>
       <c r="C13" s="25"/>
       <c r="D13" s="24"/>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="24"/>
       <c r="B14" s="25"/>
       <c r="C14" s="25"/>
       <c r="D14" s="24"/>
       <c r="E14" s="24"/>
     </row>
-    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="24"/>
       <c r="B15" s="25"/>
       <c r="C15" s="25"/>
       <c r="D15" s="24"/>
       <c r="E15" s="24"/>
     </row>
-    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="24"/>
       <c r="B16" s="25"/>
       <c r="C16" s="25"/>
       <c r="D16" s="24"/>
       <c r="E16" s="24"/>
     </row>
-    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="24"/>
       <c r="B17" s="25"/>
       <c r="C17" s="25"/>
       <c r="D17" s="24"/>
       <c r="E17" s="24"/>
     </row>
-    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="24"/>
       <c r="B18" s="25"/>
       <c r="C18" s="25"/>
@@ -1751,41 +2184,41 @@
   </sheetPr>
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="102.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="168.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="102.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="168.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="41"/>
-      <c r="E1" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="41"/>
-      <c r="I1" s="42" t="s">
+      <c r="B1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="E1" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="49"/>
+      <c r="G1" s="50"/>
+      <c r="I1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="43"/>
-    </row>
-    <row r="2" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J1" s="52"/>
+    </row>
+    <row r="2" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1795,11 +2228,11 @@
       <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="45"/>
-      <c r="G2" s="46"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="55"/>
       <c r="I2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1807,7 +2240,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -1819,12 +2252,12 @@
       </c>
       <c r="E3" s="8"/>
       <c r="G3" s="9"/>
-      <c r="I3" s="33" t="s">
+      <c r="I3" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="35"/>
-    </row>
-    <row r="4" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="57"/>
+    </row>
+    <row r="4" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>12</v>
       </c>
@@ -1850,7 +2283,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>17</v>
       </c>
@@ -1860,11 +2293,11 @@
       <c r="C5" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="34"/>
-      <c r="G5" s="35"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="57"/>
       <c r="I5" s="13" t="s">
         <v>21</v>
       </c>
@@ -1872,7 +2305,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>23</v>
       </c>
@@ -1891,12 +2324,12 @@
       <c r="G6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="33" t="s">
+      <c r="I6" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="35"/>
-    </row>
-    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J6" s="57"/>
+    </row>
+    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>29</v>
       </c>
@@ -1922,7 +2355,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E8" s="5" t="s">
         <v>34</v>
       </c>
@@ -1939,7 +2372,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E9" s="10" t="s">
         <v>38</v>
       </c>
@@ -1950,14 +2383,14 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E10" s="33" t="s">
+    <row r="10" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="34"/>
-      <c r="G10" s="35"/>
-    </row>
-    <row r="11" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F10" s="58"/>
+      <c r="G10" s="57"/>
+    </row>
+    <row r="11" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E11" s="5" t="s">
         <v>41</v>
       </c>
@@ -1968,7 +2401,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D12" s="20"/>
       <c r="E12" s="5" t="s">
         <v>44</v>
@@ -1980,13 +2413,13 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D13" s="20"/>
       <c r="E13" s="8"/>
       <c r="G13" s="9"/>
       <c r="J13" s="21"/>
     </row>
-    <row r="14" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E14" s="1" t="s">
         <v>46</v>
       </c>
@@ -1997,14 +2430,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E15" s="36" t="s">
+    <row r="15" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E15" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="37"/>
-      <c r="G15" s="38"/>
-    </row>
-    <row r="16" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F15" s="60"/>
+      <c r="G15" s="61"/>
+    </row>
+    <row r="16" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E16" s="13" t="s">
         <v>47</v>
       </c>
@@ -2015,7 +2448,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="5:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E17" s="5" t="s">
         <v>8</v>
       </c>
@@ -2026,7 +2459,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="5:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E18" s="13" t="s">
         <v>34</v>
       </c>
@@ -2037,7 +2470,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="5:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E19" s="13" t="s">
         <v>38</v>
       </c>
@@ -2048,7 +2481,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="5:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E20" s="13" t="s">
         <v>53</v>
       </c>
@@ -2059,14 +2492,14 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="5:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E21" s="36" t="s">
+    <row r="21" spans="5:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E21" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="37"/>
-      <c r="G21" s="38"/>
-    </row>
-    <row r="22" spans="5:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F21" s="60"/>
+      <c r="G21" s="61"/>
+    </row>
+    <row r="22" spans="5:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E22" s="16" t="s">
         <v>55</v>
       </c>
@@ -2079,16 +2512,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E21:G21"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="I3:J3"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E21:G21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2096,258 +2529,684 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD8DA07F-D72C-490D-8102-03B8FA54BD9C}">
-  <dimension ref="A2:V7"/>
+  <dimension ref="A1:V12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView showGridLines="0" zoomScale="72" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="17" width="12.85546875" customWidth="1"/>
-    <col min="18" max="18" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="45.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="35" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="43.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="31" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="24.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="54"/>
-      <c r="B2" s="55" t="s">
+    <row r="1" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="41"/>
+      <c r="B1" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
+      <c r="Q1" s="69"/>
+      <c r="R1" s="70"/>
+      <c r="S1" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55" t="s">
-        <v>64</v>
-      </c>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="60"/>
-      <c r="S2" s="55" t="s">
+      <c r="T1" s="63"/>
+      <c r="U1" s="63"/>
+      <c r="V1" s="63"/>
+    </row>
+    <row r="2" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="42"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="74" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="71" t="s">
+        <v>63</v>
+      </c>
+      <c r="N2" s="72"/>
+      <c r="O2" s="72"/>
+      <c r="P2" s="72"/>
+      <c r="Q2" s="72"/>
+      <c r="R2" s="73"/>
+      <c r="S2" s="65"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="66"/>
+      <c r="V2" s="66"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A3" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="T2" s="55"/>
-      <c r="U2" s="55"/>
-      <c r="V2" s="55"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="54"/>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="55" t="s">
-        <v>62</v>
-      </c>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="55"/>
-      <c r="R3" s="54"/>
-      <c r="S3" s="54"/>
-      <c r="T3" s="54"/>
-      <c r="U3" s="54"/>
-      <c r="V3" s="54"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="56" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="57" t="s">
+      <c r="G3" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="L3" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="M3" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="N3" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q3" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="R3" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="S3" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="T3" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="U3" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="V3" s="43" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A4" s="40">
+        <v>1</v>
+      </c>
+      <c r="B4" s="40" t="str" cm="1">
+        <f t="array" ref="B4:E4">_xlfn.XLOOKUP(A4,Population!$A$2:$A$18,Population!$B$2:$E$18,"")</f>
+        <v>uniform</v>
+      </c>
+      <c r="C4" s="40">
+        <v>5000</v>
+      </c>
+      <c r="D4" s="40">
+        <v>0</v>
+      </c>
+      <c r="E4" s="40">
+        <v>0</v>
+      </c>
+      <c r="F4" s="40">
+        <f>COUNTIF(Chain_Details!$A$2:$A$23, 'Scenario Overview'!A4)</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="40">
+        <v>1</v>
+      </c>
+      <c r="H4" s="40" t="e" cm="1">
+        <f t="array" ref="H4">_xlfn.XLOOKUP(1,(Chain_Details!$A$2:$A$23 = 'Scenario Overview'!A4)*(Chain_Details!$B$2:$B$23= 'Scenario Overview'!G4),Chain_Details!$C$2:$G$23)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40">
+        <v>2</v>
+      </c>
+      <c r="N4" s="40" t="str" cm="1">
+        <f t="array" ref="N4">IF(F4&gt;1,_xlfn.XLOOKUP(1,(Chain_Details!$A$2:$A$23 = 'Scenario Overview'!A4)*(Chain_Details!$B$2:$B$23= 'Scenario Overview'!G4),Chain_Details!$C$2:$G$23), "")</f>
+        <v/>
+      </c>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="40"/>
+      <c r="S4" s="40" cm="1">
+        <f t="array" ref="S4:V4">_xlfn.XLOOKUP(A4,Outbreaks!$A$2:$A$18,Outbreaks!$B$2:$E$18,"")</f>
+        <v>0.5</v>
+      </c>
+      <c r="T4" s="40">
+        <v>0.01</v>
+      </c>
+      <c r="U4" s="40">
+        <v>10</v>
+      </c>
+      <c r="V4" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A5" s="40">
+        <v>2</v>
+      </c>
+      <c r="B5" s="40" t="str" cm="1">
+        <f t="array" ref="B5:E5">_xlfn.XLOOKUP(A5,Population!$A$2:$A$18,Population!$B$2:$E$18,"")</f>
+        <v>radial_clusters</v>
+      </c>
+      <c r="C5" s="40">
+        <v>5000</v>
+      </c>
+      <c r="D5" s="40">
+        <v>0.05</v>
+      </c>
+      <c r="E5" s="40">
         <v>3</v>
       </c>
-      <c r="C4" s="56" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="58" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4" s="56" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" s="56" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4" s="57" t="s">
-        <v>60</v>
-      </c>
-      <c r="H4" s="56" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="57" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="57" t="s">
-        <v>46</v>
-      </c>
-      <c r="K4" s="56" t="s">
-        <v>48</v>
-      </c>
-      <c r="L4" s="59" t="s">
-        <v>61</v>
-      </c>
-      <c r="M4" s="57" t="s">
-        <v>60</v>
-      </c>
-      <c r="N4" s="56" t="s">
-        <v>26</v>
-      </c>
-      <c r="O4" s="57" t="s">
-        <v>14</v>
-      </c>
-      <c r="P4" s="57" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q4" s="56" t="s">
-        <v>48</v>
-      </c>
-      <c r="R4" s="59" t="s">
-        <v>61</v>
-      </c>
-      <c r="S4" s="58" t="s">
-        <v>15</v>
-      </c>
-      <c r="T4" s="58" t="s">
-        <v>21</v>
-      </c>
-      <c r="U4" s="56" t="s">
-        <v>32</v>
-      </c>
-      <c r="V4" s="56" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="54">
-        <v>1</v>
-      </c>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54">
+      <c r="F5" s="40">
         <f>COUNTIF(Chain_Details!$A$2:$A$23, 'Scenario Overview'!A5)</f>
         <v>1</v>
       </c>
-      <c r="G5" s="54" t="str">
-        <f>_xlfn.XLOOKUP(A5 &amp; "-" &amp; B2, Chain_Details!Z:Z, Chain_Details!C:C, "Not Found")</f>
-        <v>Not Found</v>
-      </c>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="54"/>
-      <c r="K5" s="54"/>
-      <c r="L5" s="54"/>
-      <c r="M5" s="54"/>
-      <c r="N5" s="54"/>
-      <c r="O5" s="54"/>
-      <c r="P5" s="54"/>
-      <c r="Q5" s="54"/>
-      <c r="R5" s="54"/>
-      <c r="S5" s="54"/>
-      <c r="T5" s="54"/>
-      <c r="U5" s="54"/>
-      <c r="V5" s="54"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="54">
+      <c r="G5" s="40">
+        <v>1</v>
+      </c>
+      <c r="H5" s="40" t="e" cm="1">
+        <f t="array" ref="H5">_xlfn.XLOOKUP(1,(Chain_Details!$A$2:$A$23 = 'Scenario Overview'!A5)*(Chain_Details!$B$2:$B$23= 'Scenario Overview'!G5),Chain_Details!$C$2:$G$23)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40">
         <v>2</v>
       </c>
-      <c r="B6" s="54"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54">
+      <c r="N5" s="40" t="str" cm="1">
+        <f t="array" ref="N5">IF(F5&gt;1,_xlfn.XLOOKUP(1,(Chain_Details!$A$2:$A$23 = 'Scenario Overview'!A5)*(Chain_Details!$B$2:$B$23= 'Scenario Overview'!G5),Chain_Details!$C$2:$G$23), "")</f>
+        <v/>
+      </c>
+      <c r="O5" s="40"/>
+      <c r="P5" s="40"/>
+      <c r="Q5" s="40"/>
+      <c r="R5" s="40"/>
+      <c r="S5" s="40" cm="1">
+        <f t="array" ref="S5:V5">_xlfn.XLOOKUP(A5,Outbreaks!$A$2:$A$18,Outbreaks!$B$2:$E$18,"")</f>
+        <v>0.5</v>
+      </c>
+      <c r="T5" s="40">
+        <v>0.01</v>
+      </c>
+      <c r="U5" s="40">
+        <v>10</v>
+      </c>
+      <c r="V5" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A6" s="40">
+        <v>3</v>
+      </c>
+      <c r="B6" s="40" t="str" cm="1">
+        <f t="array" ref="B6:E6">_xlfn.XLOOKUP(A6,Population!$A$2:$A$18,Population!$B$2:$E$18,"")</f>
+        <v>uniform</v>
+      </c>
+      <c r="C6" s="40">
+        <v>20000</v>
+      </c>
+      <c r="D6" s="40">
+        <v>0</v>
+      </c>
+      <c r="E6" s="40">
+        <v>0</v>
+      </c>
+      <c r="F6" s="40">
         <f>COUNTIF(Chain_Details!$A$2:$A$23, 'Scenario Overview'!A6)</f>
-        <v>1</v>
-      </c>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="54"/>
-      <c r="M6" s="54"/>
-      <c r="N6" s="54"/>
-      <c r="O6" s="54"/>
-      <c r="P6" s="54"/>
-      <c r="Q6" s="54"/>
-      <c r="R6" s="54"/>
-      <c r="S6" s="54"/>
-      <c r="T6" s="54"/>
-      <c r="U6" s="54"/>
-      <c r="V6" s="54"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="54">
-        <v>3</v>
-      </c>
-      <c r="B7" s="54"/>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54">
+        <v>2</v>
+      </c>
+      <c r="G6" s="40">
+        <v>1</v>
+      </c>
+      <c r="H6" s="40" t="e" cm="1">
+        <f t="array" ref="H6">_xlfn.XLOOKUP(1,(Chain_Details!$A$2:$A$23 = 'Scenario Overview'!A6)*(Chain_Details!$B$2:$B$23= 'Scenario Overview'!G6),Chain_Details!$C$2:$G$23)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40">
+        <v>2</v>
+      </c>
+      <c r="N6" s="40" t="e" cm="1">
+        <f t="array" ref="N6">IF(F6&gt;1,_xlfn.XLOOKUP(1,(Chain_Details!$A$2:$A$23 = 'Scenario Overview'!A6)*(Chain_Details!$B$2:$B$23= 'Scenario Overview'!G6),Chain_Details!$C$2:$G$23), "")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O6" s="40"/>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="40"/>
+      <c r="R6" s="40"/>
+      <c r="S6" s="40" cm="1">
+        <f t="array" ref="S6:V6">_xlfn.XLOOKUP(A6,Outbreaks!$A$2:$A$18,Outbreaks!$B$2:$E$18,"")</f>
+        <v>0.5</v>
+      </c>
+      <c r="T6" s="40">
+        <v>0.01</v>
+      </c>
+      <c r="U6" s="40">
+        <v>10</v>
+      </c>
+      <c r="V6" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A7" s="40">
+        <v>4</v>
+      </c>
+      <c r="B7" s="40" t="str" cm="1">
+        <f t="array" ref="B7:E7">_xlfn.XLOOKUP(A7,Population!$A$2:$A$18,Population!$B$2:$E$18,"")</f>
+        <v>radial_clusters</v>
+      </c>
+      <c r="C7" s="40">
+        <v>20000</v>
+      </c>
+      <c r="D7" s="40">
+        <v>2.5</v>
+      </c>
+      <c r="E7" s="40">
+        <v>5</v>
+      </c>
+      <c r="F7" s="40">
         <f>COUNTIF(Chain_Details!$A$2:$A$23, 'Scenario Overview'!A7)</f>
         <v>2</v>
       </c>
-      <c r="G7" s="54"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="54"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="54"/>
-      <c r="L7" s="54"/>
-      <c r="M7" s="54"/>
-      <c r="N7" s="54"/>
-      <c r="O7" s="54"/>
-      <c r="P7" s="54"/>
-      <c r="Q7" s="54"/>
-      <c r="R7" s="54"/>
-      <c r="S7" s="54"/>
-      <c r="T7" s="54"/>
-      <c r="U7" s="54"/>
-      <c r="V7" s="54"/>
+      <c r="G7" s="40">
+        <v>1</v>
+      </c>
+      <c r="H7" s="40" t="e" cm="1">
+        <f t="array" ref="H7">_xlfn.XLOOKUP(1,(Chain_Details!$A$2:$A$23 = 'Scenario Overview'!A7)*(Chain_Details!$B$2:$B$23= 'Scenario Overview'!G7),Chain_Details!$C$2:$G$23)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40">
+        <v>2</v>
+      </c>
+      <c r="N7" s="40" t="e" cm="1">
+        <f t="array" ref="N7">IF(F7&gt;1,_xlfn.XLOOKUP(1,(Chain_Details!$A$2:$A$23 = 'Scenario Overview'!A7)*(Chain_Details!$B$2:$B$23= 'Scenario Overview'!G7),Chain_Details!$C$2:$G$23), "")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O7" s="40"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="40"/>
+      <c r="S7" s="40" cm="1">
+        <f t="array" ref="S7:V7">_xlfn.XLOOKUP(A7,Outbreaks!$A$2:$A$18,Outbreaks!$B$2:$E$18,"")</f>
+        <v>0.5</v>
+      </c>
+      <c r="T7" s="40">
+        <v>0.01</v>
+      </c>
+      <c r="U7" s="40">
+        <v>20</v>
+      </c>
+      <c r="V7" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A8" s="40">
+        <v>5</v>
+      </c>
+      <c r="B8" s="40" t="str" cm="1">
+        <f t="array" ref="B8:E8">_xlfn.XLOOKUP(A8,Population!$A$2:$A$18,Population!$B$2:$E$18,"")</f>
+        <v>uniform</v>
+      </c>
+      <c r="C8" s="40">
+        <v>20000</v>
+      </c>
+      <c r="D8" s="40">
+        <v>0</v>
+      </c>
+      <c r="E8" s="40">
+        <v>0</v>
+      </c>
+      <c r="F8" s="40">
+        <f>COUNTIF(Chain_Details!$A$2:$A$23, 'Scenario Overview'!A8)</f>
+        <v>1</v>
+      </c>
+      <c r="G8" s="40">
+        <v>1</v>
+      </c>
+      <c r="H8" s="40" t="e" cm="1">
+        <f t="array" ref="H8">_xlfn.XLOOKUP(1,(Chain_Details!$A$2:$A$23 = 'Scenario Overview'!A8)*(Chain_Details!$B$2:$B$23= 'Scenario Overview'!G8),Chain_Details!$C$2:$G$23)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="40">
+        <v>2</v>
+      </c>
+      <c r="N8" s="40" t="str" cm="1">
+        <f t="array" ref="N8">IF(F8&gt;1,_xlfn.XLOOKUP(1,(Chain_Details!$A$2:$A$23 = 'Scenario Overview'!A8)*(Chain_Details!$B$2:$B$23= 'Scenario Overview'!G8),Chain_Details!$C$2:$G$23), "")</f>
+        <v/>
+      </c>
+      <c r="O8" s="40"/>
+      <c r="P8" s="40"/>
+      <c r="Q8" s="40"/>
+      <c r="R8" s="40"/>
+      <c r="S8" s="40" cm="1">
+        <f t="array" ref="S8:V8">_xlfn.XLOOKUP(A8,Outbreaks!$A$2:$A$18,Outbreaks!$B$2:$E$18,"")</f>
+        <v>0.5</v>
+      </c>
+      <c r="T8" s="40">
+        <v>0.01</v>
+      </c>
+      <c r="U8" s="40">
+        <v>10</v>
+      </c>
+      <c r="V8" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A9" s="40">
+        <v>6</v>
+      </c>
+      <c r="B9" s="40" t="str" cm="1">
+        <f t="array" ref="B9:E9">_xlfn.XLOOKUP(A9,Population!$A$2:$A$18,Population!$B$2:$E$18,"")</f>
+        <v>radial_clusters</v>
+      </c>
+      <c r="C9" s="40">
+        <v>20000</v>
+      </c>
+      <c r="D9" s="40">
+        <v>0.05</v>
+      </c>
+      <c r="E9" s="40">
+        <v>3</v>
+      </c>
+      <c r="F9" s="40">
+        <f>COUNTIF(Chain_Details!$A$2:$A$23, 'Scenario Overview'!A9)</f>
+        <v>2</v>
+      </c>
+      <c r="G9" s="40">
+        <v>1</v>
+      </c>
+      <c r="H9" s="40" t="e" cm="1">
+        <f t="array" ref="H9">_xlfn.XLOOKUP(1,(Chain_Details!$A$2:$A$23 = 'Scenario Overview'!A9)*(Chain_Details!$B$2:$B$23= 'Scenario Overview'!G9),Chain_Details!$C$2:$G$23)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40">
+        <v>2</v>
+      </c>
+      <c r="N9" s="40" t="e" cm="1">
+        <f t="array" ref="N9">IF(F9&gt;1,_xlfn.XLOOKUP(1,(Chain_Details!$A$2:$A$23 = 'Scenario Overview'!A9)*(Chain_Details!$B$2:$B$23= 'Scenario Overview'!G9),Chain_Details!$C$2:$G$23), "")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O9" s="40"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="40"/>
+      <c r="S9" s="40" cm="1">
+        <f t="array" ref="S9:V9">_xlfn.XLOOKUP(A9,Outbreaks!$A$2:$A$18,Outbreaks!$B$2:$E$18,"")</f>
+        <v>0.5</v>
+      </c>
+      <c r="T9" s="40">
+        <v>0.01</v>
+      </c>
+      <c r="U9" s="40">
+        <v>10</v>
+      </c>
+      <c r="V9" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A10" s="40">
+        <v>7</v>
+      </c>
+      <c r="B10" s="40" t="str" cm="1">
+        <f t="array" ref="B10:E10">_xlfn.XLOOKUP(A10,Population!$A$2:$A$18,Population!$B$2:$E$18,"")</f>
+        <v>radial_clusters</v>
+      </c>
+      <c r="C10" s="40">
+        <v>5000</v>
+      </c>
+      <c r="D10" s="40">
+        <v>2.5</v>
+      </c>
+      <c r="E10" s="40">
+        <v>3</v>
+      </c>
+      <c r="F10" s="40">
+        <f>COUNTIF(Chain_Details!$A$2:$A$23, 'Scenario Overview'!A10)</f>
+        <v>2</v>
+      </c>
+      <c r="G10" s="40">
+        <v>1</v>
+      </c>
+      <c r="H10" s="40" t="e" cm="1">
+        <f t="array" ref="H10">_xlfn.XLOOKUP(1,(Chain_Details!$A$2:$A$23 = 'Scenario Overview'!A10)*(Chain_Details!$B$2:$B$23= 'Scenario Overview'!G10),Chain_Details!$C$2:$G$23)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="40">
+        <v>2</v>
+      </c>
+      <c r="N10" s="40" t="e" cm="1">
+        <f t="array" ref="N10">IF(F10&gt;1,_xlfn.XLOOKUP(1,(Chain_Details!$A$2:$A$23 = 'Scenario Overview'!A10)*(Chain_Details!$B$2:$B$23= 'Scenario Overview'!G10),Chain_Details!$C$2:$G$23), "")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O10" s="40"/>
+      <c r="P10" s="40"/>
+      <c r="Q10" s="40"/>
+      <c r="R10" s="40"/>
+      <c r="S10" s="40" cm="1">
+        <f t="array" ref="S10:V10">_xlfn.XLOOKUP(A10,Outbreaks!$A$2:$A$18,Outbreaks!$B$2:$E$18,"")</f>
+        <v>0.5</v>
+      </c>
+      <c r="T10" s="40">
+        <v>0.01</v>
+      </c>
+      <c r="U10" s="40">
+        <v>8</v>
+      </c>
+      <c r="V10" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A11" s="40">
+        <v>8</v>
+      </c>
+      <c r="B11" s="40" t="str" cm="1">
+        <f t="array" ref="B11:E11">_xlfn.XLOOKUP(A11,Population!$A$2:$A$18,Population!$B$2:$E$18,"")</f>
+        <v>uniform</v>
+      </c>
+      <c r="C11" s="40">
+        <v>20000</v>
+      </c>
+      <c r="D11" s="40">
+        <v>0</v>
+      </c>
+      <c r="E11" s="40">
+        <v>0</v>
+      </c>
+      <c r="F11" s="40">
+        <f>COUNTIF(Chain_Details!$A$2:$A$23, 'Scenario Overview'!A11)</f>
+        <v>1</v>
+      </c>
+      <c r="G11" s="40">
+        <v>1</v>
+      </c>
+      <c r="H11" s="40" t="e" cm="1">
+        <f t="array" ref="H11">_xlfn.XLOOKUP(1,(Chain_Details!$A$2:$A$23 = 'Scenario Overview'!A11)*(Chain_Details!$B$2:$B$23= 'Scenario Overview'!G11),Chain_Details!$C$2:$G$23)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="40"/>
+      <c r="M11" s="40">
+        <v>2</v>
+      </c>
+      <c r="N11" s="40" t="str" cm="1">
+        <f t="array" ref="N11">IF(F11&gt;1,_xlfn.XLOOKUP(1,(Chain_Details!$A$2:$A$23 = 'Scenario Overview'!A11)*(Chain_Details!$B$2:$B$23= 'Scenario Overview'!G11),Chain_Details!$C$2:$G$23), "")</f>
+        <v/>
+      </c>
+      <c r="O11" s="40"/>
+      <c r="P11" s="40"/>
+      <c r="Q11" s="40"/>
+      <c r="R11" s="40"/>
+      <c r="S11" s="40" cm="1">
+        <f t="array" ref="S11:V11">_xlfn.XLOOKUP(A11,Outbreaks!$A$2:$A$18,Outbreaks!$B$2:$E$18,"")</f>
+        <v>0.5</v>
+      </c>
+      <c r="T11" s="40">
+        <v>0.01</v>
+      </c>
+      <c r="U11" s="40">
+        <v>7</v>
+      </c>
+      <c r="V11" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A12" s="40">
+        <v>9</v>
+      </c>
+      <c r="B12" s="40" t="str" cm="1">
+        <f t="array" ref="B12:E12">_xlfn.XLOOKUP(A12,Population!$A$2:$A$18,Population!$B$2:$E$18,"")</f>
+        <v>radial_clusters</v>
+      </c>
+      <c r="C12" s="40">
+        <v>20000</v>
+      </c>
+      <c r="D12" s="40">
+        <v>2.5</v>
+      </c>
+      <c r="E12" s="40">
+        <v>5</v>
+      </c>
+      <c r="F12" s="40">
+        <f>COUNTIF(Chain_Details!$A$2:$A$23, 'Scenario Overview'!A12)</f>
+        <v>1</v>
+      </c>
+      <c r="G12" s="40">
+        <v>1</v>
+      </c>
+      <c r="H12" s="40" t="e" cm="1">
+        <f t="array" ref="H12">_xlfn.XLOOKUP(1,(Chain_Details!$A$2:$A$23 = 'Scenario Overview'!A12)*(Chain_Details!$B$2:$B$23= 'Scenario Overview'!G12),Chain_Details!$C$2:$G$23)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="40">
+        <v>2</v>
+      </c>
+      <c r="N12" s="40" t="str" cm="1">
+        <f t="array" ref="N12">IF(F12&gt;1,_xlfn.XLOOKUP(1,(Chain_Details!$A$2:$A$23 = 'Scenario Overview'!A12)*(Chain_Details!$B$2:$B$23= 'Scenario Overview'!G12),Chain_Details!$C$2:$G$23), "")</f>
+        <v/>
+      </c>
+      <c r="O12" s="40"/>
+      <c r="P12" s="40"/>
+      <c r="Q12" s="40"/>
+      <c r="R12" s="40"/>
+      <c r="S12" s="40" cm="1">
+        <f t="array" ref="S12:V12">_xlfn.XLOOKUP(A12,Outbreaks!$A$2:$A$18,Outbreaks!$B$2:$E$18,"")</f>
+        <v>0.5</v>
+      </c>
+      <c r="T12" s="40">
+        <v>0.01</v>
+      </c>
+      <c r="U12" s="40">
+        <v>8</v>
+      </c>
+      <c r="V12" s="40">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="S2:V2"/>
-    <mergeCell ref="F2:Q2"/>
-    <mergeCell ref="G3:L3"/>
-    <mergeCell ref="M3:Q3"/>
+    <mergeCell ref="B1:E2"/>
+    <mergeCell ref="F1:R1"/>
+    <mergeCell ref="M2:R2"/>
+    <mergeCell ref="G2:L2"/>
+    <mergeCell ref="S1:V2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>